<commit_message>
Get daily reddit data: Tue Dec 10 08:12:10 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_15.xlsx
+++ b/data/collected_data/2024_12_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C496"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,3321 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1havg04</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Salon cut live skin when trimming cuticles, help!!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1havg04</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1hav5s8</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>I love the sparkly purple 💜 ✨</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywqw3sk6oy5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1haukzj</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Christmas Nails ✨</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6khdlolvhy5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1hau3aw</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aquarius </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bugfe1fvcy5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1hatnv9</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you use fake tip with gel polish? </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hatnv9/can_you_use_fake_tip_with_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1hatd5i</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Joining all the holiday nail posts ♥️</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azmtv9gm5y5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1hat481</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creepmas nails </t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1uc94ob53y5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1hat14s</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Christmas set with press-ons 🤗</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gf55oie2y5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1hasf3f</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Advice for at home mani?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hasf3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1harwi8</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>What is the difference?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1harwi8/what_is_the_difference/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1haru89</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>My Christmas tiny pressons😮‍💨</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haru89</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1harm7z</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>starfish nails… yay or nay ?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aova6s3yox5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1har674</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Sumer</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb37xinvkx5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1har469</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Sparkly Christmas vibes…</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1har469</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1haqwcy</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>ASP Builder and Gel x retention tips?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1haqwcy/asp_builder_and_gel_x_retention_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1haqsbo</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>colors by llarowe Final Fantasy released summer 2014</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwb8caddhx5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1haq4bi</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>christmas set!!</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haq4bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1hapfvs</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>First Christmas set! ❤️🎄</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hapfvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1hapfs4</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Starting to get into the Christmas sprite !🎄🎄</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hdzt24d5x5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1hap9r3</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>A light tone this time..</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn2nuwzw3x5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1hanz5w</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Walking on a thin line ________</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a2pysp1tw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1haougp</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>How do we feel about different colors on each hand?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haougp</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1haor2p</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Can you shape the bottom of handmade press on nails once they’re completed?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1haor2p/can_you_shape_the_bottom_of_handmade_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1haokhw</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>need to post my (grown out) nails somewhere!</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haokhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1haoi12</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Press on Nails on Painted Nails</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1haoi12/press_on_nails_on_painted_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1hao62o</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Is this color season appropriate, of course it is!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87joihjnuw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1hao0uj</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Can I reshape my acrylic nails at home?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hao0uj</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1hanw46</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Christmas Sweater Nails! 10 hours!</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5qc2khcsw5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1hant98</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Best treatment for damaged nails</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cu8hui6prw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1hakx27</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️❄️</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0qqwm635w5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1halbuc</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Ripped off my gel x in a fit of boredom in the office. What now?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1halbuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1hanhix</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Acrylic hate?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hanhix/acrylic_hate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1handrw</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mc00dh4ow5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1hamszr</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>One year of progress!</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hamszr</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1hampm6</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>set for my graduation !!!🍸</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrinlbcpiw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1hamoid</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>What do u think? too classic? 🖤</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akmdou4giw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1hamnd3</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>i got them done today, i really like them!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kjql3o6iw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1hamixt</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>What type of nail file do you use, and why do you like it?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hamixt/what_type_of_nail_file_do_you_use_and_why_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1hamgkk</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Set 🎄 </t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1pznmfpgw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1halnc4</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Does this shape look good in my nails?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1halnc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1hal3hy</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Is this lifting and what causes it?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gofoaane6w5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1hakt7w</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What am I doing wrong? </t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hakt7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1hajwau</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Holiday set on my mom 🌟🎄</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am1g2nyhxv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1hakakq</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Gel tips vs acrylics?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hakakq/gel_tips_vs_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1hak3an</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>I do my own nails at home but this Christmas set has me feeling ✨professional✨</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eq1ebhyyyv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1hajrkt</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Steam gel remover, any good?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.bask-la.com/products/lux-steam-off</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1hajh1u</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue Winter Acrylic Set❄️, But Something Feels Off lol </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hajh1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1haiooj</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How’d I do on my 13yo daughter’s nails? </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haiooj</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1hai830</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Time with Cat Gel! </t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z4vvhlo4lv5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1hahrqs</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Need some sparkly holiday inspo for short nails</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hahrqs/need_some_sparkly_holiday_inspo_for_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1hahkg6</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Gave my nail tech free reign! Very happy</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hahkg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1hah6g8</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Manicure 💅</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hah6g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1hah0fd</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tiny bows </t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31y5m4cacv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1haguje</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Finished painting the Arcane Logo for my Jinx Nail Set ☺️🩵🩷 not used to writing AAAAA</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9uzxp83bv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1hagnvz</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Blue chrome for Christmas 💙</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/coer4ltq9v5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1hagkmf</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Full plastic nails? Pros &amp; cons?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hagkmf/full_plastic_nails_pros_cons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1hagk1m</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>holiday set ❄️</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hagk1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1hagfkl</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Finally finished a set for a gift 🥹 Super proud of myself but also kind of unhappy with them at the same time! 😭</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yb9ax4v7v5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1hag8vs</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What should I do with my nails? </t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hag8vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1hafsl7</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>First time doing Gel X!</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hafsl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1hafrn6</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Latest set! Absolutely love 💗 </t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1e213aa3v5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1hafnfb</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas nails. </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hafnfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1hafj4v</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Ready for christmas</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t4t40al1v5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1hafa8y</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple nails for Christmas </t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcy1yhttzu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1haf8wv</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Loving my holiday nails.</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abwr6huizu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1haeyzj</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>My Christmas set 🎀</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypd4nw0jxu5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1hael03</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>I just peeled off my last mani...</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hael03/i_just_peeled_off_my_last_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1haek2w</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>My nail keeps breaking in the same spot, what can I do to prevent this?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haek2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1haeipc</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Second set of Christmas nails!!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8b2yco8uu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1haeiiv</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Christmas pedi</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cgmns16uu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1hadeg9</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmassy set </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0g1msqxlu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1haddc8</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did these myself first time trying anything like this </t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haddc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1h9vwvk</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Blue cat eye, not sure if i love them</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h9vwvk/blue_cat_eye_not_sure_if_i_love_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1h9x3pr</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>My work in a trade I did with another tech! Recreation of @nst.notgi on ig :)</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9x3pr</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1h9zmfn</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is HEMA free polish safe to prevent an allergy? </t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h9zmfn/is_hema_free_polish_safe_to_prevent_an_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ha2w29</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Ok y’all im gonna do my own gel x nails at home. What do I need?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ha2w29/ok_yall_im_gonna_do_my_own_gel_x_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ha6avm</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clown Nails for friend 🤡 </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mza71flfos5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1had0du</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Nail shape?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkfizvpziu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1hacja3</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Tips</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hacja3/tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ha9y4y</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas set 🎄 </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m2t0xzvttt5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ha6txe</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Never gotten my nails done professionally before. What should I expect?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ha6txe/never_gotten_my_nails_done_professionally_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1hacs13</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>My Christmas nails</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muf43yl9hu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1hacq8j</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">☺️ Happy Holidays!!! </t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfun40ltgu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1hac0xp</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Help with press on nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hac0xp/help_with_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1habu22</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1jfaowo9u5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1haaxin</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>new basic but lovely set 🥰</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/einjjbwc2u5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1haafki</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Which Nail Shape Suits Me Better?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haafki</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1haaapp</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Which Nail Shape Suits Me Better?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haaapp</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1ha9txb</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Holiday nails 🎄</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w74j6kist5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1ha9kud</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Had my nails done for the first time 😍</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha9kud</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1ha9hwl</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What brand of paper forms do you recommend? </t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ha9hwl/what_brand_of_paper_forms_do_you_recommend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1ha89b3</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first acrylic set i did myself </t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha89b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1ha87ln</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>I just love nail art so much 💕</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha87ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1ha6yj2</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Recommendations for a broken nail</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onmb83dixs5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1ha6xtf</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>What do you guys think? ($25USD!!!)</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha6xtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ha6iq5</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha6iq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ha6fs2</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljrfxjkeqs5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ha5qxu</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Dip powder?</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ha5qxu/dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ha5meo</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Christmas set🎄✨️</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha5meo</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1ha5kpq</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This Christmas I opted for shorts nails and a little glitter. What do you think? </t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g44gb5v7es5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1hawbsg</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Love the shift on this! 💙</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hawbsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1havr7k</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Trying out nail art</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vc9kg1k7vy5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1haval4</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">follow my beauty page 🩷🩷 </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/bel.lasbeautybar/profilecard/?igsh=MTcyZDFxbG1nM3V2aA==</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1hav92l</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>follow my beauty instagram 🩷🩷🩷</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hav92l/follow_my_beauty_instagram/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1haudp5</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Obsessed with this pink 😍</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g37ii28rfy5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1hatyer</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Polish Organization Systems</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hatyer/polish_organization_systems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1hats5k</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>How do you use toppers?</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2y582f3q9y5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1hat5i8</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>My first Christmas set I've done so far this year!</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hat5i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1hast04</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New colours </t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hast04</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1hasquz</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Icy blue nails from my BKL Black Friday haul</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hasquz</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1hasman</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>KINDNESS WITH CRACKED</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7qwy31dyx5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1hascci</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My manicure lasted through a move! </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzct30hovx5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1has5kx</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Tis the season 🎄⭐️</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1has5kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1has0p9</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Best nail polish removal tool? I use acetone on regular polish, but Walgreens "improved" my favorite cotton rounds which used to have woven string in them.</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1has0p9/best_nail_polish_removal_tool_i_use_acetone_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1harc20</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Psilocybin being crazy + I need tips on magnetization </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1harc20</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1har4rv</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hyponychium like detached from nail bc I filed my nail way down. Any tips to make it less painful? </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1har4rv/hyponychium_like_detached_from_nail_bc_i_filed_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1har0v5</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Broken nail &amp; press-ons </t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcf8vwzijx5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1haqrzx</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>colors by llarowe Final Fantasy released summer 2014</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfrqangahx5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1haqb0z</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blade of the Frontiers </t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haqb0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1hapqct</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>UK nail polish thinner recommendations?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hapqct/uk_nail_polish_thinner_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1hapnkg</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Please recommend me base and top coats!!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hapnkg/please_recommend_me_base_and_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1hap3jq</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>First attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hap3jq</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1haombp</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Accidentally cut my toenail way too short</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcuuxieeyw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1haoadp</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Does anyone actually use backup polishes?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1haoadp/does_anyone_actually_use_backup_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1hanp23</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Can you help me find a nail polish with this color?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5k28hwzqqw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1hanifn</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Someone asked if this color was season appropriate...</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovlw1ge7pw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1hamsoy</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Seche Vive on top of Seche Vite</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hamsoy/seche_vive_on_top_of_seche_vite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1hamsns</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas glitter ✨ </t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfrj2qfejw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1hamlgg</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Nail Buffer Replacement?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hamlgg/nail_buffer_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1halv2s</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>When your Black Friday order finally gets it</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/im03i847cw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1halp61</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Multi-chrome Skittles </t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ofxce7yaw5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1halc00</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>wedding mani ❤️</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1halc00</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1hal7m3</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Can someone help me find these shades?? (For a cosplay but yeah..)</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbwkxu0a7w5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1hal601</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Birthday mani</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91sh4xpx6w5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1hakogc</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Adding "two drops of thinner" to a nearly deceased polish...</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwvdjjca3w5e1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1hak1nq</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Too many steps in DIY builder gel?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyvhnxpmyv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1hajvh4</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>I don't have any Christmas polishes so I had to improvise.</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bic6cdqbxv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1hajlmu</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Curse Mark</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jy309r79vv5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1haji2f</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Sweater Mani</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cz4arajuv5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1hajbj9</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Subtle or non-contrasting shimmers?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hajbj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1haiq1o</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Two manis today ? Why not 🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haiq1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1haipxu</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Two manis today ? Why not 🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haipxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1haifb4</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Tried a new salon - the pup approves!</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9amgbckmmv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1hai5zw</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Christmas paper stamping</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hai5zw</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1hah585</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Anyone else use toppers on unflattering colors to make them more appealing?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4w2g2ye7dv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1hah0ja</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Is consignment polish “safe”?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n32fcuracv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1hagira</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Thermals are so fun on long nails 😱</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hagira</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1hag925</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>(Yet another) ILNP Overcast skittle 🌧️</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hag925</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1hag5n8</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Candy cane anyone? </t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hag5n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1hag4yu</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today's nails </t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hag4yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1haf4di</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Shiny Christmas tips</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haf4di</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1haek05</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail polish storage journey &amp; review of the Bisley 6 drawer unit as an alternative to Ikea's Helmer! </t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haek05</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1haefmk</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Help with streaking?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haefmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1haeetm</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>How can I achieve this look at home?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rjhurcitu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1haed7k</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is one of, if not THE most fun &amp; unique glitters I own </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gou3sav7tu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1hadu85</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>It’s a sad day</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hadu85</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1hadlcx</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Has anyone else used Monarch’s gel effect top coat?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hadlcx/has_anyone_else_used_monarchs_gel_effect_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1had5vg</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Mooncat’s Garden of Evil 😍</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1had5vg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1haclio</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Is this shape flattering on me?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcfa4uusfu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1hacgci</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>The Many Faces of a Magnetic Skittle</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hacgci</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1hace3m</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Anyone taking good nail photos on an iPhone 13 Mini? Or, do you love the 16?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hace3m/anyone_taking_good_nail_photos_on_an_iphone_13/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1hac7ve</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>A Spot in the Woods is my new favorite polish</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urmjp9brcu5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1hac6nl</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Is any top coat is good enough?? Chipping and denting on DAY ONE...</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hac6nl/is_any_top_coat_is_good_enough_chipping_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1habsr9</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Very impressed with ILNP’s gorgeous metallics</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2l2yz63f9u5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1habriq</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>New to nails longer than my fingertips. How do you all grate things?</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1habriq/new_to_nails_longer_than_my_fingertips_how_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1habd1g</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>UPDATE Husband-Made (Nail) Polish Advent</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34zs129z5u5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1haar4x</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Beautiful Grey</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haar4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1haadcs</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Hema free (cat eye) gel polish brand favourites?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1haadcs/hema_free_cat_eye_gel_polish_brand_favourites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1ha9b3s</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Flakie gradient</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha9b3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ha988s</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Matchin’ with my festive doggo 🎄</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha988s</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ha94he</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Queen of the dead</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha94he</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1h9zc5v</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swatch Storing Recommendations  </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h9zc5v/swatch_storing_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1ha79zi</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ha79zi/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1ha6v1d</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Trying on my “untrieds” part 1</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha6v1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1ha6npk</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Adding saturation to Holo Taco's OG Cristmas glitters (plus a birthstone dupe!)</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha6npk</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1hav3rz</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>In 7 years of practice I’ve never been so proud of a set. All handpainted on myself 💅🏼</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hav3rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1hauert</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>pls help me pick my next nail set 🫶‼️</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hauert/pls_help_me_pick_my_next_nail_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1hatw9o</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>First set of acrylics I did myself!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hatw9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1haryx2</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just doing some practice </t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xwx3e7q9sx5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1hargxs</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>New manicure with cat-eye gems—love it!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hargxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1haq48z</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opinions/constructive criticism please! </t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haq48z</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1hap5y0</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting into the Christmas sprite 🎄🤶🏻 </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7qkfh913x5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1haoxvd</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Christmas set using stamping plates</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haoxvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1haogd4</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>1st time ever trying any sort of nail art!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cprsb7zww5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1haod8v</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gabriela Rodriguez </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nsehuh7bww5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1hamdz4</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Opinions ?</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hamdz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1haix5q</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Wicked!</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haix5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1haim3n</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Holiday set</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aahoiyq1ov5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1hahtcl</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter is coming and gold is a perfect match </t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hahtcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1hagutu</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Finished painting the Arcane Logo for my Jinx Nail Set ☺️🩵🩷</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t62fjbf5bv5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1haemwj</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Pastel Xmas Nails</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haemwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1haatms</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Autumn!!!! 😍</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rly8ljbg1u5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ha9v7u</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>ARCANE / JINX NAIL ART - Let me know what you think!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ha9v7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ha7cgb</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Goldfish Nails</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jhwb21c2t5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1ha5m4f</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Glass Skies nail art tutorial</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5k66ivrres5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Dec 11 08:11:46 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_15.xlsx
+++ b/data/collected_data/2024_12_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C496"/>
+  <dimension ref="A1:C682"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8866,6 +8866,3168 @@
         </is>
       </c>
     </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1hbomlk</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas baubles and snowflakes ❄️ </t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbomlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1hbo77q</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>I feel so basic while looking at the posts here but hey, here it is Arcane Jinx nails 💅</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r3yyxil866e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1hbnj9n</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>I have a habit of not only chewing my press-ons, but also the nail glue underneath once it falls off. Am I in genuine danger?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbnj9n/i_have_a_habit_of_not_only_chewing_my_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1hbn57y</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Tis the season ❄️♥️</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udogul1dv56e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1hbn1lj</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suggestions to rebuild growth and strength </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbn1lj</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1hbl68b</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Sticky tab press ons</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbl68b/sticky_tab_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1hbmv7f</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Holiday nails! 💚❤️</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69oayqq4s56e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1hbmta4</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Where to find this color from The Gel Bottle?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v87qbyiir56e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1hbmdm0</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>I love shiny nails and you?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m03jdhim56e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1hbm4ww</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed, photoshoot in the grocery store </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbm4ww</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1hblv4z</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Interesting form</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c02tpqnpg56e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1hblqwa</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m sad </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orl335s1g56e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1hbkxvn</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Christmas 🎄 Nails</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jmt86mw756e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1hbkp9y</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Builder Gel for my holiday nails</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbkp9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1hbkmyb</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Neutral Tones</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbkmyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1hbkgw0</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Of the most beautiful and tender nails I’ve ever made, what do you think? </t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbkgw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1hbjt7k</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Cracked Acrylic AND Real Nail. What Do I do?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbjt7k/cracked_acrylic_and_real_nail_what_do_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1hbk4ml</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to Acrylics </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbk4ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1hbk4gf</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to Acrylics </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbk4gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1hbjoxr</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>How can I fix these?? 😭</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2d33qzzzv46e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1hbjmiw</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black french </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bhva3idv46e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1hbi8wt</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Where can i get large quantities of UV nail gel without breaking the bank?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbi8wt/where_can_i_get_large_quantities_of_uv_nail_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1hbhxah</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Red Velvet 🎄</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2p1zfsvf46e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1hbhtof</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendations - guy clear matt finish - AUstralia </t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbhtof/recommendations_guy_clear_matt_finish_australia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1hbhmo6</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Is this an air bubble?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbhmo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1hbhjkx</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas set 🎄 </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbhjkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1hbhgcd</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>I think it looks like snow!</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osy57z7rb46e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1hbhe67</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red nails are such a vibe. </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbhe67</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1hbh0wq</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>UPDATE on the giant spoon nails</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbh0wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1hbh4ja</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Nice new glue lol</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75v035cv846e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1hbgtrl</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Gradient stamping</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbgtrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1hbgo05</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>In love with the result, what do you think?😍💅💖</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg56ccyv446e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1hbgk69</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Classic nails ☺️ definitely love them 😍</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbgk69</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1hbfnd6</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Aura Nails 💜</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbfnd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1hbfko3</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Recent nails I’ve done on others :)</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbfko3</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1hbfesj</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Is there such a thing as form-fitting reusable gloves for gel polish?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbfesj/is_there_such_a_thing_as_formfitting_reusable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1hbfbfm</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh December Set ❄️ </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agmwrvirt36e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1hbfb5t</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gimme Christmas but make it dark and moody. You got it! </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbfb5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1hbeg0c</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail advice? </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbeg0c/nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1hbev2k</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love the poof </t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbev2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1hbenrh</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>We are fresh 💅</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixug3ccgo36e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1hbemdv</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>I'm just a girl 🙂‍↔️🎀</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn3lz8j7o36e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1hbea43</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural or gel extensions? </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbea43</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1hbe1nv</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Man’s nails (Christmas edition) </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbe1nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1hbe0ue</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>As a Male How do I file/trim my nails as they grow out without raising a lot of attention?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbe0ue</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1hbdm7u</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love that gel polish so much </t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbdm7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1hbd5ne</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>So proud of this set and it being my favourite character?!?! Was so fun to replicate the art style 🥰🫶🏼</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbd5ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1hbczt3</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Perfect nails to start 2025 with?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbczt3/perfect_nails_to_start_2025_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1hbcult</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Holiday Set</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fm9aj7ba36e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1hbbvf5</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Reusable press-ons - need glue remover that won't damage nail polish/art</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbbvf5/reusable_pressons_need_glue_remover_that_wont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1hbcgp4</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>My Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu2b667d736e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1hbbs34</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>which shape looks better on me</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbbs34</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1hbboq7</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Just had my nails done for the first time!!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbboq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1hbbaoh</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Just got into school and need some beginner tips!</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbbaoh/just_got_into_school_and_need_some_beginner_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1hbb913</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Podiatrist’s suggestions for treating damaged toenail matrix</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbb913/podiatrists_suggestions_for_treating_damaged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1hbavjc</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Xmas 2024</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbavjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1hbar3s</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>How short can I get my nails?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcz2wtpku26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1hbadya</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>The great almond vs whatever else shape debate</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbadya</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1hbab01</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Odd shape on side profile of nails </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g83jyfk6r26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1hba39y</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gold Double French for Christmas </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hba39y</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1hb9xhh</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>My cousin 💅🏼my nails</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb9xhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1hb9mj8</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Dip Nails </t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb9mj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1hb9lso</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first attempt at butterfly nails! </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb9lso</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1hb9h3d</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>My first time doing my own gel nails. How did I do?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78zbnvmyk26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1hb9a5v</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First post, hello everyone! </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb9a5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1hb9871</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Apex method with builder gel</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6w3ook6j26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1hb8ywe</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Finished X-Mas Set</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb8ywe</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1hb8yrc</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>christmas nails 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/octdx6b7h26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1hb8i3t</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas X Arcane nails </t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/399lcr1td26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1hb8sqx</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Swooning…</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lvlx7nzf26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1hb8s11</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Last set of the year…💬</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb8s11</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1hb8o5r</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Not sure how I feel about the shape, but still happy that they look so clean 😌</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sknmu5t0f26e1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1hb8k89</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Didn’t think I’d be this happy going green instead of red💚</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5m1mv68e26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1hb7rav</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Should I get my (potentially engagement) nails redone?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb7rav</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1hb7x6s</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Help please</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hb7x6s/help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1hb67c2</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspo pic from @kaitlynbandaid4 from Pinterest. Need a good colour match </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2ydt3tmw16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1hb7249</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Confused on the acrylic process. Which one do I choose?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hb7249/confused_on_the_acrylic_process_which_one_do_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1hb77qn</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do i have press on nail blindness? </t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9aqjvrk6426e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1hb6vum</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another set of press ons! </t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb6vum</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1hb6sn9</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>first set i’ve ever done on my myself</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssobnsh1126e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1hb6ehi</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Do professional pedicures/manicures always paint your nails?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hb6ehi/do_professional_pedicuresmanicures_always_paint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1hb6aci</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Getting in to the holiday spirit, thoughts??????</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/siyy0rr9x16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1hb5ul8</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Christmas set 🎄❤️💖</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcgmccmxt16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1hb5nss</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>My failed attempt at perfect sharp squares 😞</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cutgs0zgs16e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1hb5fgw</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Red wine/arterial/cherry color?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb5fgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1hb5ewg</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Deformed nail</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smj6tqokq16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1hb59vt</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday Nails 🎂 </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb59vt</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1hb4zf1</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Christmas Tree Cakes 🎄</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1te1lqan16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1hasllw</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Discoloration </t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxrxi006yx5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1haseq7</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Looking for top coat recommendations!</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1haseq7/looking_for_top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1hav4lu</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Curved nails</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hav4lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1hawggq</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">There are so many options on how to do your nails at home, which is the best? </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hawggq/there_are_so_many_options_on_how_to_do_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1haxpwc</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is going on with my nails after using builder gel </t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haxpwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1hb0v6t</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Finally figured out I was allergic to the base and top coat I was using</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2f9yrc32o06e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1hb1cu4</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Took a break from acrylic and my nails have never looked worse😭</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tz4ifbvs06e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1hb1uuk</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Salon etiquette for first time?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hb1uuk/salon_etiquette_for_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1hb1vkn</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Burgundy 😍</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mxpjo1dsx06e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1hb2lw5</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want to try press on nails but .. </t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8x7xm893416e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1hb3d52</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Recovered Nail biter. I keep them so long now, my little trophies.</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb3d52</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1hb4kt9</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>red nails for the christmas season</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3k5d6qq1k16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1hbo9i4</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>2 month old acrylic nail fell off last week and yesterday half of my natural nail fell off and exposed the skin underneath… Why did this happend and can I avoid this in the future?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oedkdudg966e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1hbmm79</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Looking for top coat recommendations! From a gel allergic girlie...</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbmm79/looking_for_top_coat_recommendations_from_a_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1hbm2bt</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Wicked - defying gravity magnetic?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3z7il68j56e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1hbltvs</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Festive Green</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0lmgslvg56e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1hbln7x</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Finally put it on</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04euya7ze56e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1hbl43i</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Help with purple dupes?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3k5z2gdm956e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1hbl1fo</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alien Life Form 👽 </t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbl1fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1hbjokr</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>First gel! I like the color but could use some advice on getting the edges to be neat!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbjokr</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1hbjlps</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Holo Taco Hot Wire Pink vs Mooncat Venus Flytrap</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbjlps/holo_taco_hot_wire_pink_vs_mooncat_venus_flytrap/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1hbjarg</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Subtle jelly skittle</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbjarg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1hbj2qu</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Mery Crimis</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbj2qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1hbgl0w</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>PSA: if you haven't already, you should layer your ILNP Bluebell and Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shlaqsg5446e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1hbfq0r</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>When both bf orders arrive on the same day😍</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbfq0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1hbfpem</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Trouvaille</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbfpem</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1hbfokm</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Aura Nails 💜</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbfokm</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1hbfmst</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>really loving this colour 🥺 I call it rose quartz pink 🩷</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trad0k1dw36e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1hbfejv</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LOVE Mooncat, but for people who haven't seen magnetic thermals before... </t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aob9dx5xt36e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1hbez4i</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>“Northern Exposure” 🌲🫎🌨️</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbez4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1hbeps6</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Using seche restore question</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbeps6/using_seche_restore_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1hbelgn</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>How do you remove someone else’s nail polish without messing up your own manicure?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbelgn/how_do_you_remove_someone_elses_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1hbd0bw</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Deeply unhappy with Cirque Magnets</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbd0bw/deeply_unhappy_with_cirque_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1hbcxe3</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">📷 💅 Sassy sauce. Featuring a surprise admirer. </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbcxe3</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1hbchzc</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>German Laqueristas: I'd love some advice about acrylic services in Germany. Please point me in the right direction, friends &lt;3</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbchzc/german_laqueristas_id_love_some_advice_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1hbc2q5</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>✨️🍭Rainbow Candy🍭✨️</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbc2q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1hbbxp9</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Ghosts of Christmas </t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbbxp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1hbbqyw</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>ISO the perfect cornflower blue</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4qouwd2236e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1hbbl1j</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Dupe Suggestions for Ard As Nails’ "Now He's A Philosophizer" from February 2024 Polish Pickup? 🙏</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbbisb</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1hbbg6v</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>ILNP Petals 🌺</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ywo53ptz26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1hbaizq</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>First magnetic polish and first ILNP polish 🧲</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbaizq</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1hb9ycj</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Mooncat moonrise vs ILNP flower child</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hb9ycj/mooncat_moonrise_vs_ilnp_flower_child/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1hb9foi</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>One month difference!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb9foi</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1hb91ps</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>L.A. Colors?! Pop off💚</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ic8i3yth26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1hb8rir</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>My skittle from Mooncat BF order</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb8rir</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1hb8qn9</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>[Swatch Request] Could someone please end my suffering? (HT vs. ILNP)</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hb8qn9/swatch_request_could_someone_please_end_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1hb875b</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Holiday ready!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb875b</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1hb86vw</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>2025 Color of the Year</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5ac26zgb26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1hb7vg4</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>A Lil' Something Extra</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb7vg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1hb79wp</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Blue nails for December🩵</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb79wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1hb78kg</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Psilocybin by the Seaside</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfb6fpcd426e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1hb767x</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>These shifts are insane</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb767x</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1hb6ylb</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking to sell polish. What brands sell well? </t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hb6ylb/looking_to_sell_polish_what_brands_sell_well/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1hb6ver</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>nov 11th - dec 10th growth</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb6ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1hb5xtq</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Obsessed with my Wicked nail art 💅</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb5xtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1hb5uqx</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's a Fall-Nomenon </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb5uqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1hb5shv</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Husband's required reaction for new polish</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg0t5vkht16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1hb5rep</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>This lil guy makes me so happy</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rrgg9t8t16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1hb5pdt</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Moderately festive shorties ✨</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb0y1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1hb585f</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Kbshimmer Aft Backwards</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb585f</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1hb4zyr</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>You Hooooo!!! 🗣️</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp7mblsen16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1hb4ytf</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>it’s tiiiiiiime 🔔🎁🎄</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb4ytf</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1hb4gdl</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried. </t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q508hat5j16e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1hb4604</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Swatched my first ILNP Order 😍</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb4604</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1hb3zzw</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>New glitter combo</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb3zzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1hb3sjg</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Anchor &amp; Heart Lacquer - over three weeks and not shipped. Is this normal? I've never purchased from them before.</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hb3sjg/anchor_heart_lacquer_over_three_weeks_and_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1hb2lmo</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP “Charmed” and the top and bottom coat are amazing even if I still need to finish cleaning up my nails. </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb2lmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1hb2iq5</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Spoilers for Emily de Molly and Rogue Lacquer’s Advent Calendars</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb2iq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1hb1x5k</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Root of All Evil</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb1x5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1hb1tlx</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HT Rainbow Snow vs Ride or Diamond? </t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hb1tlx/ht_rainbow_snow_vs_ride_or_diamond/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1hazmn2</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>ISO hema-free gels in the EU</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hazmn2/iso_hemafree_gels_in_the_eu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1hazakq</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hazakq/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1haythw</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s definitely the season to break this one out </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0zkrab8006e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1haqa8s</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>The Natural Nail Journey Begins… Advice?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1haqa8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1hawp7y</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Color comparison: Zoya Ryder and Orly Yeah, for Sherpa</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hawp7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1hawspt</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>ILNP Pyro vs Flicker</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hawspt</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1hboq9k</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>astarion-themed press-ons🩸🗡️</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hboq9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1hbmgzl</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>You like this style?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lii6136ln56e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1hbkkej</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Neutral Tones</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbkkej</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1hbkdu7</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Pros are beautiful, cons are inconvenient.</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbkdu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1hbjwak</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>What's missing?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afiybpprx46e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1hbjqyx</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Krampus Nails</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqrizmrjw46e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1hbj3pd</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>I did it again @streetnail.art</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4czjj8kkq46e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1hbeckc</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to do this? </t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0occtzhzl36e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1hbe2qr</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sculpting gel? </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hbe2qr/sculpting_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1hbdv8n</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>What is this trend called?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5us9g8d5i36e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1hbdtoj</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vyk652th36e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1hbdnvt</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Todays set!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p96xx1bkg36e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1hbddxg</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>How long does it take to get good at nail art?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hbddxg/how_long_does_it_take_to_get_good_at_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1hbd59f</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally Finished My Jinx Nail Set! *They are stuck on over my XL acrylics as I have a Christmas event tomorrow 🥰 hence them not being flush to the cuticle or align with my knuckle! </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbd59f</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1hbbcdm</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Cherry😍</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1w8yf7w1z26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1hbadqx</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>ocean theme press ons</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3cxzxkrr26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1hb8gbg</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Eras nails minus one</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srxhc1fdd26e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1hb7hgl</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Pink and Red Christmas 💖🎄</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr6swzh8626e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1hb79cd</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gabriela Rodriguez </t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05ai6t5j426e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1hb6rx7</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>My Frozen Christmas Set by my magical nail tech @nails_emmywynn on IG ❄️⛄️</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0v3rjew026e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1hb6mu9</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Tis the season</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb6mu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1hb63pu</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did my own nails </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb63pu</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Dec 12 08:11:55 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_15.xlsx
+++ b/data/collected_data/2024_12_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C682"/>
+  <dimension ref="A1:C874"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12028,6 +12028,3270 @@
         </is>
       </c>
     </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1hcfmb4</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Would you try these WEARABLE SOAKING DEVICES to enhance your manicure/pedicure routine?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1esgbo69ad6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1hcdvyt</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Do my nails look a little too long?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcdvyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1hcf48h</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>New nails! Inspired by My dress up darling!</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9orfrcj84d6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1hcf1gb</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>tis the season 🎄</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcf1gb</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1hcet8s</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">V excited about these. </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcet8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1hcekjk</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🥳</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcekjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1hcejge</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>My nail stylist really outdid herself this time</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcejge</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1hcedck</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Holiday Velvet Cat-eye Set</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5am5d94gvc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1hcebsy</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t like my pinky nail. What could have been better? </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nv5kagoyuc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1hce9z5</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Recreation of Elphaba's Nails</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hce9z5</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1hcdwf9</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting Acrylics for the first time </t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hcdwf9/getting_acrylics_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1hcdv6l</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Natural length</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrjjv1tppc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1hcdhsh</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Gel x or acrylic for newbie</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hcdhsh/gel_x_or_acrylic_for_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1hcd4ca</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Blue Nails for my Engagment Pictures 💙🩵</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcd4ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1hcczes</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Wanted to show off my amazing catholic gothic vampire esqe nails</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4xlv9bkgc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1hccmee</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Nails are ready for the holidays♥️🎄🎁</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rb9u8xsvcc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1hccl3o</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Broken nail</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hifyk5ehcc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1hcc9c8</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Christmas Nails 💚🎄</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39rhdcm59c6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1hcci71</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Christmas stickers!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcci71</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1hcc43o</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So glad I found this sub. My last set! </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0bbmkep7c6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1hcbtjx</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcbtjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1hcbs94</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Pink winter nails!!</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3q89p4dg4c6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1hcbroy</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at French Tips </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcbroy</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1hcbqli</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Christmas vibes nails 💚🤍</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvao3szz3c6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1hcbh6w</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made cute winter nails </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0ujj7mi1c6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1hcb0oz</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>UV Lamp for multiple brands of gel?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hcb0oz/uv_lamp_for_multiple_brands_of_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1hc8d88</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>how would i fix this?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6j8thff9b6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1hcbems</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail artists!!! how much should this be??? </t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ik0wzept0c6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1hcazh5</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>What can I do for my nail?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0odf2m1ywb6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1hcb7g7</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nail set made by myself </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqiywwuzyb6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1hcamyi</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>DIY pidgeon-themed set</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcamyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1hcat67</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Holiday themed!!</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcat67</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1hcan2h</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Simple holiday chrome tip</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcan2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1hc9lu7</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You’re a mean one Mr Grinch </t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc9lu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1hc9i5o</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Icy / sparkly / silver winter nails! 🧊 ❄️ 🥶🩵🌐🪩</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc9i5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1hc9hj2</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Got a new fill for winter. ❄️🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33v2a3xajb6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1hc956r</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Feeling a little Blue</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hc956r/feeling_a_little_blue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1hc90in</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Update to my wife’s vacay nails!</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vn8p2t4fb6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1hc8ty9</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>What nail glue and nail glue remover should I buy?</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hc8ty9/what_nail_glue_and_nail_glue_remover_should_i_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1hc8kz3</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How did I do? Is this a good shape for my fingers? </t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oev86rabbb6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1hc83to</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Loving the short press ons for this busy time of the year!🤍</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxqdygi77b6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1hc7tmx</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Merry Christmas 🎅🏻</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc7tmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1hc7h20</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why are gel x so much more expensive than acrylic/ sns? </t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hc7h20/why_are_gel_x_so_much_more_expensive_than_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1hc764l</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>The first set I’m actually happy with…</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc764l</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1hc78fl</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Sassy Saints - eye irritation</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc78fl</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1hc7afn</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>new design just done. what do you think?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc7afn</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1hc651f</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>NOTHING has stopped my peeling nails and I'm desperate. Please help!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc651f</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1hc6xh1</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>nothing beats the magic of cat eye imo</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sulijm45xa6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1hc6lm5</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Beary cute😍🐻</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1q0j8qkua6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1hc6l9g</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t xml:space="preserve">did a new gel X set! any advice is welcome </t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc6l9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1hc67dv</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Fixing gel polish ?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hc67dv/fixing_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1hc64al</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails 💅 🎄 </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qf1unz7sqa6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1hc6223</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>New set of sharp sparkly French ombré nails</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc6223</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1hc5r94</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Quick pink glitter jellies.</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcgch9txna6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1hc5qno</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>To cut or not to cut ...</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc5qno</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1hc57ug</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone asked where I got my nails done </t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ubxzkhuja6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1hc5755</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>First attempt at cracked ice nails</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc5755</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1hc519s</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Did my own gel nails. How/what can i improve ?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc519s</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1hc4q46</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Feeling ✨festive✨</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e27z5pbyfa6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1hc45xn</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>candy cane nails!!!!</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp9sjaeoba6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1hc41vj</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>How often do you need to get a new set?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hc41vj/how_often_do_you_need_to_get_a_new_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1hc3qz0</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Are my nails as bad as I think?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc3qz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1hc3hqj</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>On a scale of 1-10, how natural do these press ons look?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc3hqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1hc3124</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chanel le vernis 125 Muse </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc3124</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1hc2zbr</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Christmas Nails with some Peppermint Flair! 🍬🎄</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc2zbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1hc2xb4</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Fun and festive</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfjh7v3e2a6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1hc2lnp</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Elvis Nails (inspo: @nailnova on ig)</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hx4enuaxz96e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1hc2kcj</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Neonails „pre base quick off“</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hc2kcj/neonails_pre_base_quick_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1hc2de2</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Gingerbread nails 😋</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc2de2</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1hc2bvf</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Electronic Nail File</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpdkj9a0y96e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1hc1zpt</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Did my bestie and my nails</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc1zpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1hc1vob</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Can you grow your nails long when you have a job that has you working with your hands?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hc1vob/can_you_grow_your_nails_long_when_you_have_a_job/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1hc1eiy</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Giving your nails a rest?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hc1eiy/giving_your_nails_a_rest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1hc1alr</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgd3f7aaq96e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1hc0x6i</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>My 2 weeks old nails</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xg5gcyjn96e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1hc022k</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I need guidance 🙈</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hc022k/i_need_guidance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1hc0jwx</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m all in on Xmas this year </t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc0jwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1hc086b</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail removal for the first time </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/975l0n7fi96e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1hbzvtb</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice (male 18). </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbzvtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1hbzpr5</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>almond, square or coffin?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbzpr5/almond_square_or_coffin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1hbzgsq</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Nail progress!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbzgsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1hbyvok</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nail tutorial, how they look? </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8oi3bn5i896e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1hbvv41</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Ideas for engagement nails</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbvv41/ideas_for_engagement_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1hbyaf7</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Weak nails after overdoing them</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbyaf7/weak_nails_after_overdoing_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1hbwgew</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>today I have a nude matte manicure with a little glitter</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ih0iz06eq86e1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1hbs5h0</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyway i can fix this? the guy who did my nails told me i have to cut it and wait for it to grow back. It's my natural nails and gel </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6szrh6neo76e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1hbtxoc</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prep Question </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbtxoc/prep_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1hbvjt3</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Nail Polish Peeling Help!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbvjt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1hbw3eo</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Accidentally touched dry pasta with wet polish</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbw3eo/accidentally_touched_dry_pasta_with_wet_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1hbv4bx</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>My nail tech is awful!! Left a large amount of glue on my hands</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lst54wxf86e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1hbv3g8</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wife got her nails done for vacation and I’m kind of obsessed 😍 </t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5rnx4vqf86e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1hbuqzy</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First chrome 🧡 </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7de03rqc86e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1hbupep</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>I wanted to paint xmas nails for the Christmas market but only had time for one hand...</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uyl7w7ec86e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1hbuap0</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Red French Santa hat nails 🎅🏼</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbuap0</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1hbt7iv</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>ILNP - Someday</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbt7iv</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1hbssl3</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue collar guy, trying to stay a little goth </t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nc9sca2pu76e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1hbs0rb</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just home use and getting there.. just love French polish and a Christmas touch.. </t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbs0rb</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1hbru6d</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Second time doing my own nails. In love with this builder gel color. What other colors do you think would look good on me?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbru6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1hbrm9a</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>🎄🤶🎁🎅🎄</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/957ajs3fi76e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1hbqqiw</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Prep advice</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hbqqiw/prep_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1hcg4v3</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>What are your favorite snowy, wintry, glowy, sparkly, flakey polishes? White, off-white, or blue</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hcg4v3/what_are_your_favorite_snowy_wintry_glowy_sparkly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1hcg4lu</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can someone help me with my nails? </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcg4lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1hcfg79</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cracked polish 23 flavors </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x12pnt5o8d6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1hcfe12</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Help with cirque colors</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hcfe12/help_with_cirque_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1hce754</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I know I’m late to the party but… </t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b63cwh0gtc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1hcdfcj</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Where to buy dazzle dry in Canada?🫶🏻</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hcdfcj/where_to_buy_dazzle_dry_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1hcd24b</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Cheat code for magnetics</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcd24b</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1hcczol</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Dupe request: Scotch Naturals “Klondike Cooler”</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcczol</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1hcccho</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>i have a humble color request</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2k2h2zu1ac6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1hcbfdg</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Happy B-day to me!</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s8n6mmfv0c6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1hcb6og</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Please help me fix my nails I have zero knowledge on self-care</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcb6og</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1hcawfq</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving ‘on the rocks’ by ILNP </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcawfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1hcatvq</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>ILNP Mega (with flash) 😍✨</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4on0bk4cvb6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1hcatr3</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Bluebell</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcatr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1hcardz</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Holiday Themed!!</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcardz</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1hcaclw</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>You NEED Mani Mags! Velvet Perfection 10/10</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nffgul53rb6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1hca0vy</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>❄️🧚‍♀️✨️ vibes</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hca0vy</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1hc9xst</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Maybe my last fall mani before I switch to winter colors</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc9xst</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1hc9ruj</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Topper Tuesday</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f31o83tu036e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1hc9nrd</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat - Shroomdom </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8c8hwyrkb6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1hc99uw</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Begonia nails</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc99uw</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1hc925a</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Sydney CBD Stores?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hc925a/sydney_cbd_stores/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1hc8sle</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Holo taco BF order 💿🌮</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc8sle</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1hc8rzx</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Orly shimmers</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hc8rzx/orly_shimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1hc8nzj</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>We got a picture with the god of war</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7re7912cb6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1hc8i6l</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No idea anymore if these are nice or disgusting... </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc8i6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1hc8108</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Glowy Holiday Mani!</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc8108</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1hc7hqq</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>The Black Friday bonus from Bee's Knees Lacquer with the BG3 collection 😆</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxo1if2w1b6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1hc7f9g</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>First time wearing Cirque Colors’s Sol</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc7f9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1hc77ql</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Y’all doing any faux sneaux manis?🤍❄️</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mqgmfxxfza6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1hc7377</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>🦋butterfly🦋</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc7377</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1hc72hr</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Magnetic topper reccomendations</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hc72hr/magnetic_topper_reccomendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1hc6mup</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>If you're a glitter fiend, Starrily's "Christmas Lights" is back</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8aw0w4lnua6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1hc656o</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Canada post strike</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avvufuzyqa6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1hc63yh</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>My Holo Taco BF order finally came ☺️</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b87scs8pqa6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1hc6261</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>What do you all think of lights lacquer?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gi7206vaqa6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1hc5sov</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Atomic Polish “Terraforming Mars”</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc5sov</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1hc4mow</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Possible solution to Sally Hansen's Insta-Dri Top Coat </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc4mow</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1hc44cz</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me decide tonight's nail </t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5x0wp0cba6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1hc3lxx</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>So this happened . . . .</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc3lxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1hc3ifl</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Santa con ready</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc3ifl</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1hc2okk</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long ship time from Dany Vianna? </t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hc2okk/long_ship_time_from_dany_vianna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1hc2efw</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Better brushes for ILNP polish?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30xgxlgjy96e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1hc0xi3</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>My first magnetic polish experience</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ufwp0almn96e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1hc0xho</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>I attempted a cateye with a ring magnet</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc0xho</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1hc0007</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Guilded Pink Christmas</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc0007</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1hbzea2</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Had a dream about a multichrome spaceship last night and now I want more multichrome polish. Your recommendations?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbzea2/had_a_dream_about_a_multichrome_spaceship_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1hbzbro</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Embers</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbzbro</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1hbyyig</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Chipping/Peeling Issue - Base &amp; Top Coat Recs Needed!</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbyyig</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1hbyup2</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>How to get nail polish to stick to nails better?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbyup2/how_to_get_nail_polish_to_stick_to_nails_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1hbyacf</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>first ilnp experience gone PERFECT🩷🩷</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbyacf</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1hby6vj</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Mandela Effect with ILNP bundle</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hby6vj/mandela_effect_with_ilnp_bundle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1hbxt1o</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m so glad I learned to do my own nails, I get to look down every time and think yep I did that! </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbxt1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1hbxb81</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Tardis dupe</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbxb81</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1hbwmlx</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Formulation issue or application error?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1r5kemur86e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1hbwjfw</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Jewel Beetle 🪲 So PRETTY 😍 </t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbwjfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1hbw6x6</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Nourish Your Nails: Top 6 Foods According to Dietitians</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbw6x6/nourish_your_nails_top_6_foods_according_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1hbw2po</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>fresh holographic shattered glass set by me</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbw2po</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1hbw0gs</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chipping after 1 day.. </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbw0gs</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1hbv4am</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Christmas Nails for my work party! 🎄</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbv4am</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1hbu9ex</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Polished for days Elektra is so ugly 🥲</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/28n30m03886e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1hbt94d</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Blade of the Frontiers from Bees Knees Laquers is *chefs kiss*</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbt94d</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1hbt7s4</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>ILNP - Someday</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbt7s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1hbt3eo</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Peeling nails - why do people recommend you file it out?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbt3eo/peeling_nails_why_do_people_recommend_you_file_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1hbswou</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Goal for the year....</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbswou</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1hbsndn</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Can't work- distracted by mani🥺</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tm584rot76e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1hbseem</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Shaking my sugarplums </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbseem</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1hbsana</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>I need advice please im scared</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbsana/i_need_advice_please_im_scared/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1hbrmpl</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Christmas skittle</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq1x0fbki76e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1hbqolp</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Favorite sparkly/shimmery white?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbqolp/favorite_sparklyshimmery_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1hbqku3</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Workplace Holiday Nailart Contest Entry 🌲 🎅🏻 ❄️ </t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbqku3</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1hbq7qm</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>My lacquer journey</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hbq7qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1hb8wjc</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Recs for “cat eye” gel polish?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hb8wjc/recs_for_cat_eye_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1hb9vwc</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Mojo JoJo super villain</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hb9vwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1hbm48y</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Does DND regular nail lacquer contain hema?</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbm48y/does_dnd_regular_nail_lacquer_contain_hema/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1hbpnvu</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>I just can't stay away from the reds</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbpnvu/i_just_cant_stay_away_from_the_reds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1hcdewk</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Merry Christmas!!! ☃️</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcdewk</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1hcd2wm</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Handpainted winter/Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ih089unjhc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1hccpk1</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Attempting some realism! Any tips to make it more dynamic? </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdnwft9qdc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1hccico</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Saw these nails on tiktok</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7o5r8y1qbc6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1hcb7kt</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Random lines are also artistic :p</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hcb7kt/random_lines_are_also_artistic_p/</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1hcb3v6</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>@Zulaysnails</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pjxibi2yb6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1hcamdp</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>DIY pidgeon themed set</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcamdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1hcaaur</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Christmas time</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6pms358nqb6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1hc9gf3</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did My Nails They Are Suppose To Look Like The Pressons I Made (I only did the design not the acrylic) First Time On Myself </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc9gf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1hc7myf</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Arcane jinx nails by me ✨</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc7myf</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1hc72g1</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>I like it</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc72g1</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1hc5sbd</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Christmas Nail Polish Art!</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k99s49b5oa6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1hc4tgt</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Must be jelly cause jam don't shake</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hc4tgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1hby4bk</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>🥹🥹</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muiuzuf1396e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1hbwn1w</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing acrylic nails! I think I did okay! </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjmsvl7yr86e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1hbvfx6</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkly Christmas nails </t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9rc2yffi86e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Dec 13 08:11:41 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_15.xlsx
+++ b/data/collected_data/2024_12_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C874"/>
+  <dimension ref="A1:C1060"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15292,6 +15292,3168 @@
         </is>
       </c>
     </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1hd7nok</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Red with a touch of gold 🌲✨</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb7rrj8bqk6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1hd6j68</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving red nails </t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd6j68</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1hd6inq</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Do you think these look abit kiddy &gt;.&lt; x</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eojzu5z3bk6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1hd6gok</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seaglass Nails </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q5k430xeak6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1hd6a6z</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails Broke? </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd6a6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1hd5wgi</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Chrome with neon pink this month 🎀</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7lvn7ok3k6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1hd5hh5</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd5hh5</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1hd5g7j</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flower Power </t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd5g7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1hd4tt5</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>I got my nails done in a new place. Opinions?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd4tt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1hd4sg1</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>I just got my first pedicure ever and I am new to this. How can I make my nails healthy?  More in description</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ml6cyr8frj6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1hd4jrx</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New design </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd4jrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1hd4aze</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Pretty nails for winters ❄️✨</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd4aze</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1hd3cag</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Is it possible to get gel/acrylic off without much damage?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hd3cag/is_it_possible_to_get_gelacrylic_off_without_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1hd1bj5</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice with hard skin on my pointer finger. </t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hd1bj5/advice_with_hard_skin_on_my_pointer_finger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1hd1r49</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>These nails were SO FUN to create!</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd1r49</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1hd351c</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Low watt lamp on high watt product</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hd351c/low_watt_lamp_on_high_watt_product/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1hd36eo</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>First time getting nails done in a while</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd36eo</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1hd35cd</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking at builder gel extensions </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hd35cd/looking_at_builder_gel_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1hd2zba</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Christmas Set 🎄🎅🏻</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amgqng6a9j6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1hd2vzt</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>This week's pink Christmas</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tn7i2lkd8j6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1hd2vhb</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling festive </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xe2fhg88j6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1hd2dfg</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Just wanted kawaii nails :')</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pklxp70i3j6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1hd2bvl</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got the prettiest manicure of my life done in Tokyo! </t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd2bvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1hd28c3</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GelX as a nurse? </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hd28c3/gelx_as_a_nurse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1hd21mb</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Giving Holiday Cheer </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9ywytig0j6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1hd1y2s</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>I tried</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd1y2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1hd1grv</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These are supposed to be coffin </t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd1grv</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1hd1glp</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape is this? </t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd1glp</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1hd0yom</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>First time getting Gel-X!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06ojrr5eqi6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1hd0ev2</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>what should i do for the remaining 2 press ons 👀</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzeb9gklli6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1hd0s1y</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Have you ever?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y05upruuoi6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1hd02tg</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Gel x nails issue?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd02tg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1hd011t</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>When to get a fill in?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4t5s3x5ii6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1hd00vt</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Base colour mistake?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrjo3lh4ii6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1hczntz</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>My Christmas Set!</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hczntz</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1hcznd3</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>This picture has been all over Reddit so I tried to recreate it - What do you think? ❄️</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcznd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1hczghb</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter ❄️ </t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvokh9p5di6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1hcz0j4</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Ridiculously cute nail art by my amazing tech 🎄</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcz0j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1hcyvxf</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Holiday cats 😻</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcyvxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1hcypz4</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>What style of nails should I do?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/so2dxmbv6i6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1hcy437</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">20 year long nail biter </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcy437</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1hcxe9r</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nails growing fast or user error? </t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcxe9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1hcxm4q</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Obsessed with brown</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcxm4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1hcwx4b</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Simple nude. How'd I do?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcwx4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1hcwk5t</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Craziest nails I've done 😆🙌🏻 (very impractical, but pretty) </t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcwk5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1hcvsde</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>My first Christmas set!</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcvsde</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1hcu6qy</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails before my Mexico trip </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcu6qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1hcutfb</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second set for the Christmas/winter season </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcutfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1hcvk9t</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>I love the combination of nude pink and gold, do you prefer gold or silver?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zs176tt6hh6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1hcum9c</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>First time doing Gel X nails. What do you think?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mvodrs8ah6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1hcuaiu</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>how can i improve??</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcuaiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1hcu3db</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>My Trans Nails for Early Christmas Season 🎄</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/36xds0iv5h6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1hctyjv</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>how do we feel about this color?</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hctyjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1hcty4u</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My holiday nails </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcty4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1hctb5h</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Once again my girl has killed it </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hctb5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1hcsp2o</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>How do these look? Trying to learn to do them myself, advice welcome!</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdaj2mv9vg6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1hcryby</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>My Christmas set ❄️</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcryby</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1hcrv22</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Beautiful pink hand nails to match my toenails</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ikzkdnvog6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1hcrqdq</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Soft gels. What do you think?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85pa0j11og6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1hcrjd7</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>New color shining 🩶</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3736nisimg6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1hcqn4d</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>struggling to figure out why my gel polish is not lasting</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hcqn4d/struggling_to_figure_out_why_my_gel_polish_is_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1hcr0ds</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Christmas time 🎄</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcr0ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1hcqe66</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Nail kit help</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hcqe66/nail_kit_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1hcqcrz</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Just a touch of Chrome</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcqcrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1hcqcr3</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Before, after, 5 days later</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcqcr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1hcpxs7</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think I’ve outdone myself with this set </t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcpxs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1hcpwxz</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press Ons </t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hcpwxz/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1hcpmin</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>subtle xmas nails 🫡❣️</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcpmin</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1hcpjlp</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Please rate them nails</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sndsfjrj7g6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1hcpa0k</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>One day I'll learn how to take pictures of my nails... Doing a trial run of my wedding nails for January and I'm so excited at how these turned out!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcpa0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1hcp4w8</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Arcane X Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcp4w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1hcox0z</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>My birthday nails from my birthday (which I forgot to post here)</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxxy7vrj2g6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1hcorfe</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>It’s timeeee 🎄🥹</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcorfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1hcokh4</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Mandatory Christmas Mani</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2677z4avzf6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1hckljy</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>I'm really happy with these nails</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5imkqk1k1f6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1hco04u</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Inspired by u/RachDMC! Festive mushrooms 🍄</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hco04u</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1hclroz</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Latest set, inspired by the nutcracker ballet</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3i1zfmrmcf6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1hcmcjg</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with Kokoist for a newbie? </t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hcmcjg/help_with_kokoist_for_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1hcm69l</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Please help me find this top coat!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcm69l</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1hcnckq</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>I can’t stop staring!</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gc7h6oy4qf6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1hcn8am</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>🩵❄️🩷</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcn8am</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1hcn4f6</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>half past nude (mani muse)</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcn4f6</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1hcmva8</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Winter ❄️ Nails</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uom4r579mf6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1hcmte3</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>These are blue/grey in the dark and green/ gold cat eye in the light 🙈</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcmte3</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1hcm9gz</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Holiday 2021 - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcm9gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1hclsmm</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Sweet Holiday Set</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfgcwgzucf6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1hckxk3</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Best picture I've ever taken of my nails 🌌✨</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0lwbhzr4f6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1hckg06</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>I love polka dots ⚫️⚪️</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmi1wvl00f6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1hckabc</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When you have the purrfect background </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hckabc</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1hck1bn</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Candy Cane Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckcup7irve6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1hcjwfz</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Great shape!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wu6vqvx0ue6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1hcjbc7</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Christmas nails :)</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pnu3xjpne6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1hcitwx</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner attempt at Glittery Pearl Nails </t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcitwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1hci1yx</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye Butterfly </t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p65e2q668e6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1hci0u0</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Textured fruit </t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaz1rhhr7e6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1hchslv</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best set I've done so far </t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czjxkjyq4e6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1hch9vk</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Simple Christmas bow</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uil6lmefxd6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1hch7e0</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did gel nail polish first time </t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hch7e0</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1hcgt1w</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In Honor of my Daughter who loved a good Christmas outfit </t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pz7z1h8wqd6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1hd7cq6</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Keep square or do oval nails?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd7cq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1hd751v</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Playing with Magnetics and Jellies 💖</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rxfszul6jk6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1hd6mqz</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Has anyone tried “Black Magic” by Starrily?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hd6mqz/has_anyone_tried_black_magic_by_starrily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1hd4zmd</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Tips from a newbie</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4ifo2ohtj6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1hd3u68</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Orly x ILNP</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bg961hphj6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1hd3285</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Sassy Sauce + ILNP Combo</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd3285</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1hd2qdh</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Excuse me while I stare at my nails for the next week</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o8gz111v6j6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1hd2kjf</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reflective dream </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd2kjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1hd2hsz</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>DIY softish white chrome effect</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82gbox0o4j6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1hd2hke</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Attempted a snowflake mani…they are…abstract 😂</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gi0a4dpl4j6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1hd1xqv</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>so tired of winter already so i did a spring/summery skittle!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd1xqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1hd1tcp</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I almost wish I bought a 4th bottle just for these pretty boxes! </t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd1tcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1hd1n1z</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Letting my basic flag fly</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eh30cpnqwi6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1hd1jrg</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>It was finally sunny today 😍</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ysnbnylyvi6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1hd1g37</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>ILNP Impressed!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd1g37</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1hd11cy</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Super happy with this Christmas combo 🎄</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd11cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1hd021p</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>it’s like having ten little gifts on the tips of my fingys 🤓</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f58wukdfii6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1hczwmc</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Take Me To Your Leader and Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/Lcx7jgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1hczq0v</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Update on the beetle-esque polish recs!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0b3uwqfffi6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1hcyyyr</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>I love nail polish so much omg! 😍🎄</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcyyyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1hcyke0</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BF haul came in the mail! Now to figure out what I want to use first </t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbuk6tzh5i6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1hcy6xg</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>My Black Friday BKL order came!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcy6xg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1hcy5s2</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>first holiday nails of the season! ❤️🤍</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcy5s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1hcxwba</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>fields of lavender 🪻❣️</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k1t9qdoszh6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1hcwgvn</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Clionadh forest flame</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66aumri9oh6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1hcw2qf</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>ILNP Skye (M) &amp; Elsa Accent</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ow2gmjn6lh6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1hcvm7q</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Grinch Nails!</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcvm7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1hcvlk3</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Feelin’ purple 💜</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcvlk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1hcv7iz</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Went on the hunt for the lightest green I could find ☘️</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4meh44peh6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1hcuzkn</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at a classic French tip, is the base too pink? </t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcuzkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1hcun5f</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Yes it’s just magnetic Fairy Dust, but it’s worth it!</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9zu5krv8ah6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1hcu3u5</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter art on petite nails ❄️ </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28z673p76h6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1hctmr1</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>This is definitely a favorite</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hctmr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1hctil3</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>I also got a husband-made advent this week!!!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hctil3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1hct5eh</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>My first magnetic!!</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgzzc5htyg6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1hcsimf</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Holo Taco Unicorn Skin toppers</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hcsimf/holo_taco_unicorn_skin_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1hcsar4</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Soooo sparkly</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2vk7gpgbsg6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1hcril9</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do UV reactive polishes have diminished color-changing abilities with time like thermal polishes? </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hcril9/do_uv_reactive_polishes_have_diminished/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1hcrf9v</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Holiday Party nail</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvy0l6bnlg6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1hcqffn</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Can’t Stop Chipping or Peeling in Sheets</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hcqffn/cant_stop_chipping_or_peeling_in_sheets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1hcpzqz</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>✨️❤️Glitter Candy Canes🤍✨️</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcpzqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1hcozg1</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Threw Folie a Deux on top of Serpents of Eden</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcozg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1hcoi5i</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>The Dark Urge</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcoi5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1hco1ya</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>white monster energy inspired</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v41fh1avvf6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1hcnp58</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sky Dancer </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b271psuzsf6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1hcnklb</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me find this polish! </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6emtyooyrf6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1hcngg9</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Where to put cuticle oil?!?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1ye97b0rf6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1hcnaya</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>ILNP - Merlot</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/grgrb25spf6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1hcmxnj</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where did you learn to apply nail color? </t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hcmxnj/where_did_you_learn_to_apply_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1hcmr9t</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Black Holo Wish</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3zyoyaalf6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1hcmjcb</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Such a moody color</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcmjcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1hcltm4</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zoya black friday order might not ship until after Christmas </t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hcltm4/zoya_black_friday_order_might_not_ship_until/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1hcli55</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Loving these Lurid shades together!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eubpcvhx9f6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1hckxta</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Old polish love! </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hckxta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1hckbr3</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Are these too much for a funeral?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0cec3oxtye6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1hck5jn</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Nails I’ve done on myself for the last 2 months, all with regular nail polish 🫧</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hck5jn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1hck0r8</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Twinkly fairy light nails! Not my usually style but I really like them</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zaujsnvlve6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1hcjdi2</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>I feel like my nails are out of this world</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcjdi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1hcjdgf</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Fairy Dust (ILNP) as a topper</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>/r/ILNP/comments/1hc0mfn/fairy_dust_as_a_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1hcj9q3</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t xml:space="preserve">photos absolutely do not do this one justice </t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcj9q3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1hchjz2</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>My first time being seduced by a nail polish</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hchjz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1hchegt</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Stayed up way too late to try my first ILNP order 🤩🫠😴</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hchegt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1hbtzts</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Dazzle Dry vs Manucurist</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hbtzts/dazzle_dry_vs_manucurist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1hc4yfq</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Color out of space (Essie layering)</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bs5v1inoha6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1hcgxr4</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>First time cleaning up polish with a brush, how'd I do?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwjw1tissd6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1hcgsqq</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Ah so i just noticed this important info on the bees knees site....weeks after i placed my order .....</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6peygonqd6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1hcgsnh</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>L.A. Colors Haul!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcgsnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1hd7agg</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>some holiday-ish ? stilettos 🥀⭐️🖤</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofernc1dlk6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1hd6a77</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Doflamingo themed nails I painted for my Halloween costume!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd6a77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1hd5q0f</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Any ideas ??</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd5q0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1hd5fio</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Christmas nails, beginner need adive</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd5fio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1hd4nsc</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Recently took up painting nails</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd4nsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1hd1psi</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>What would you like to be gifted for Christmas?</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hd1psi/what_would_you_like_to_be_gifted_for_christmas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1hd0ff9</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Sculptural nails!!!! 🫶</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd0ff9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1hd00gw</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>First set on someone other than my boyfriend!</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd00gw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1hcuqa8</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>💅🏼</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtt8ape4bh6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1hcuohp</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first two Christmas/winter sets of the season. </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcuohp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1hcspqa</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel and Ink Mixing </t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hcspqa/gel_and_ink_mixing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1hcsip3</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Festive vibes at the office! 🎄</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1efiv4extg6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1hcnucl</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>white monster drink inspired set</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3ew8gm6uf6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1hcng5i</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Smokey Skull</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9tiawuxqf6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1hcmuqr</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>I’m obsessed with this cat eye polish 😻</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcmuqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1hcm85u</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Holiday 2021 - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcm85u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1hcm7en</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Latest set of press on nails</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl36brjfgf6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1hcks4n</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opinion on nail artist </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hcks4n/opinion_on_nail_artist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1hchsoo</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Foil help.</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hchsoo/foil_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1hchiyw</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Christmas inspired nails</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hchiyw</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Dec 14 08:10:04 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_15.xlsx
+++ b/data/collected_data/2024_12_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1060"/>
+  <dimension ref="A1:C1260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18454,6 +18454,3406 @@
         </is>
       </c>
     </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1hdvulu</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Help!! Clear bonder gel everywhere!!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdvulu/help_clear_bonder_gel_everywhere/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1hdxzxn</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>I’m a wizard</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kq30osmrr6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1hdxghs</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>My nail tech is fantastic and puts up with me saying ‘nailed it’ literally like thirty times an appointment. A Christmas blessing</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdxghs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1hdxayy</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lots of firsts for today’s set </t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ntagenkir6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1hdxag2</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What base coat do you use? </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdxag2/what_base_coat_do_you_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1hdwe09</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hardened toenail cuticle </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfnr10kg7r6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1hdwdnu</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Manicurist polish turned purple</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ho0ba8c7r6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1hdw057</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>New nails!!!</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdw057</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1hdvsdz</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Some of my favorites this year! 💕💅🏻</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdvsdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1hdvrrd</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using press on nails! </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scrcfkqf0r6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1hdvgcb</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t xml:space="preserve">‘Tia the season </t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lz63h5yzwq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1hdvg45</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Holiday nails 🎁</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va05bqexwq6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1hdv9vu</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">graduation set </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uzpbygnyuq6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1hdv0xw</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Holiday nail ideas?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27d6uge8sq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1hdunuq</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>✨Holiday Nails✨</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z58slt0eoq6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1hduagz</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Did press ons</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adh2lmqjkq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1hdu0y6</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Snowflakes!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83yrnsduhq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1hdtvwn</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is for the OP who is getting over anxiety of being a male with painted nails. </t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdtvwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1hdtuyr</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glow in the Dark Nails </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2f5qqn45gq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1hdtr7e</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>My favourite season ❄️</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hi4bm62fq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1hdtmcr</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ca192qpdq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1hdtbs0</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blooming snow flower (all flowers are handmade) </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/be2q6r5taq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1hdt3o2</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Do I NEED to get a fill every other week?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zls6x88k8q6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1hdsap0</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Stopped biting my nails… what should i do with them?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdsap0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1hdksqz</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Consistency</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdksqz/consistency/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1hdnrad</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>How to reduce breakage/make nail polish last longer?</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdnrad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1hdo4z4</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Christmas inspired nails!</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdo4z4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1hdrarb</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just did my second set of acrylic nails on myself. </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdrarb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1hds6ru</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Getting over the (self induced) anxiety of being a guy with nails painted</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81ck4nrmzp6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1hds3z5</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>💅🏽 Pokémon themed nails</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hds3z5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1hds1mn</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Milky nails on point </t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfdvoz39yp6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1hdqwa7</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Opinions Please</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdqwa7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1hdqmv5</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Holiday Vacay Nails</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdqmv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1hdq5et</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Neutral girly </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/957jprbxgp6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1hdpuef</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>is this a crack in just the gel or also the nail?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdpuef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1hdpg03</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love blue nails </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frs6hi5sap6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1hdpfaj</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting out of my comfort zone </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ow6rztemap6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1hdpbr7</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/weyh9qas9p6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1hdp81f</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Burgundy 😍 (diy)</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7a3950cv8p6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1hdp4m2</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Rosy Nails</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ww23tf228p6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1hdp0dx</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black and red nails </t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90acow227p6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1hdozdy</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">We looove Barbie pink nails </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/or0fo6gt6p6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1hdox86</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>My holiday nails🎄</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdox86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1hdowmy</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Short blue nails💙</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3occ7956p6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1hdov8x</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🌹</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4q5a5lds5p6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1hdorap</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love how these turned out </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p973o4oy4p6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1hdook4</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>What do you think about my new nails?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arrt09jb4p6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1hdoh8r</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech sleigh-ed! </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t09faybk2p6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1hdnw2o</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Are these crap?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nq2mlkmxo6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1hdn2pt</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Winter framed ❄️🌲</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nva547b1ro6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1hdlq0h</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Acrylic woes</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdlq0h/acrylic_woes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1hdmbgi</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple xmas frenchies </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ql5dkdwko6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1hdm8j8</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Happy with my subtle Crimbus set!</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdm8j8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1hdm7cs</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Dragon Nails</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdm7cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1hdlqgq</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Tis the season</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdlqgq/tis_the_season/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1hdlnf2</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>I Made My First (good) Nails Design</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nesfvsyjfo6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1hdlesz</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Nude Christmas press ons</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ldi5xfldo6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1hdl5mo</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something about the color red 💅 </t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86g8qh8kbo6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1hdl5g8</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails always get me in the spirit </t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/whcibzribo6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1hdkybo</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>new nails 💅</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdkybo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1hdkr8y</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Christmas Nails 💅🏾❤️💚</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bc8l46p28o6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1hdk7rq</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>How can I protect my fragile nails?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdk7rq/how_can_i_protect_my_fragile_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1hdkn6p</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7ycou5f7o6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1hdjxk0</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Help me pick my next holiday set! Inspo from @nailswshey, @aleksandra_jaworskaa, @sylwia.ka_1982, @angiegutierrez_bellezayestetic, and @nailsbyauroram</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdjxk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1hdkdlc</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Holiday Nails!</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdkdlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1hdk76v</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I rarely get nail art- but I love my Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdk76v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1hdk640</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>my manicure for christmas!</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdk640</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1hdjz5e</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry nails! </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by9r83132o6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1hdjvf4</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>DIY nails after 6 months</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4ehg0n91o6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1hdjqjm</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My girl did so good on these! Probably the best holiday nails I’ve ever had ☺️🎄 </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u0moqn60o6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1hdjl99</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Awful color match</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7gysde1zn6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1hdil36</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Love how these turned out!</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdil36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1hdi3r2</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Getting ready for christmas</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3d08j2wnnn6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1hdhx9x</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Cat eye nails for December</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2z3cwp8mn6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1hdhx32</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>First set of the season!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdhx32</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1hdhnr2</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdhnr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1hdhjbw</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>First Christmas set of the year!🎅🏼☃️💅🏼</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5b6ujj6jn6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1hdh311</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Just put these on (i have short nails)</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdh311</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1hdgok0</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glass cat eye 😻 </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdgok0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1hdgkch</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Before I finish these, what’s wrong with them? </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kn6wzx5nbn6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1hdggwm</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Shape?? 💖💖</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdggwm/shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1hdgayo</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Abstract Design</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdgayo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1hdgaxf</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Subtle Christmas nails this year</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ruekso4m9n6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1hdg6kt</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Love this brown so much 🤎</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdg6kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1hdg2ab</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄🎀</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bb7nl9uo7n6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1hdft8o</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>2024 Nail roundup 💝</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdft8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1hdfi4w</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm just a straight guy wearing the colors of the season. </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tw169lz93n6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1hdfgbo</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI funny bunny and bubble bath regular polish </t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6vetkbv2n6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1hdffte</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>First Set in a Longgg Time… Holiday Nails 🎄✨</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85hkyw1s2n6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1hdf6b3</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Some recents!</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdf6b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1hdf38m</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Kiss Press On!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdf38m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1hdexwl</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Christmas Nails🎄</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdexwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1hded03</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Squoval?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hded03/squoval/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1hcu543</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This nail keeps splitting just next to the edge. Need advice </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1u1xq5496h6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1hdagyd</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>What is this called and how do I shape it?</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdagyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1hdcvp6</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>I cant get my nails healthy! Whats going on!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdcvp6/i_cant_get_my_nails_healthy_whats_going_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1hd7k4o</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don’t want to sound like a fool at the salon </t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hd7k4o/dont_want_to_sound_like_a_fool_at_the_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1hdbt4c</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manicure newb </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdbt4c/manicure_newb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1hdcrc9</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Onycholysis on both hand</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdcrc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1hddi3k</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hddi3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1hdy3dt</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Which polish looks the best on my skin ?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmr456dwsr6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1hdxtdj</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>You know her. You love her. It's Girl Dragon.</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdxtdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1hdxh93</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Winter is near…</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdxh93</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1hdx7mu</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>ISO green microshimmer topper</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdx7mu/iso_green_microshimmer_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1hdw96c</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Holiday nails ❤️🤍💚</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdw96c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1hdw3kf</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas, chrome, and mismatched hands. </t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdw3kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1hdvuin</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Pale pink creme with lilac glitter topper</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/color-cosmetic-number-10-4R75auN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1hdvn6s</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>How does this happen?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nboxho5zyq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1hdvf96</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Another Abstract</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdvf96</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1hdv526</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Definitely thought I was too late to get the free glitter. Thanks KBShimmer! </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98ldk50htq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1hduxrr</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update on the BKL EU Situation, such a Relief! </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bdeon09rq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1hduhs5</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>First LynB polish</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hduhs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1hduefk</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>as silly as this may sound, does anyone have a color suggestion to match this expo marker?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5myfb6qlq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1hduc31</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Holiday mani</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ptcxaj0lq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1hdtnrc</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>nails for a friend 🩵🩷</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdtnrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1hdt4x3</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>The Speed of the Sound of Loneliness 💜</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqrxei4x8q6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1hdt2hd</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Creeps</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2ul07198q6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1hdt0mu</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Replacing Collection After Gel Allergy Pt 2</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdt0mu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1hdst77</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rainbow reflective glitter is my new fav! </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdst77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1hdsh7h</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Don't buy shade duplicates, do this instead.</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdsh7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1hdsf3i</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Dazzle dry alternative?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdsf3i/dazzle_dry_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1hds87b</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Sheer pinks (my new boring fav)</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpo0qvduzp6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1hds5db</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please Hype Me Up </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hds5db</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1hdrab7</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Was told 4 years ago to stop wearing glitter polish in order to be taken seriously in STEM. Today I formally received my PhD</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdrab7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1hdr4e5</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Cozy and cute</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdr4e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1hdqp5t</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When the sun leaves </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdqp5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1hdqjhl</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>✨✨</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdqjhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1hdq8fy</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Got my Sassy Sauce BF haul today!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93qr0nenhp6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1hdpjaq</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>OPI - I Pink It's Snowing</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v9oe82ekbp6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1hdpanq</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>What are your favorite shifty/glowy/iridescent polishes that are stunning even indoors?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdpanq/what_are_your_favorite_shiftyglowyiridescent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1hdoy8q</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>KBShimmer BF Haul</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdoy8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1hdoq59</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Well I’m obsessed with this now</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j76rnmap4p6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1hdokdo</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Too long!</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdokdo/too_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1hdogt7</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Nursing a broken nail but my Holo Taco BF Haul came in today! 🥲🤩</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0xwgrog2p6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1hdoeiu</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Throwback vibes</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdoeiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1hdoabh</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Blue polish is the best polish 😍</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdoabh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1hdnpet</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Can you get an allergy doing normal enamel polish at home?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdnpet/can_you_get_an_allergy_doing_normal_enamel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1hdnjjm</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mermaid nails! </t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdnjjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1hdnbv5</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Photo dump of me entering my magnetic polish era🧲✨ feat: Fancy Gloss “Space Hydra” and “Space Gnome”</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdn9yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1hdnbd0</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Cleaning a magnetic want with acetone?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdnbd0/cleaning_a_magnetic_want_with_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1hdn9xz</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s Showtime! by BKL, living up to my own hype. </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdn9xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1hdn8b6</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>What nail/nail polish opinions have you done a 180 on?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdn8b6/what_nailnail_polish_opinions_have_you_done_a_180/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1hdn2cv</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Mistook remover for solvent and now I pay the price.</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdn2cv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1hdmqkd</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Candy cane nails and my furry helper 🎅🏻🐾</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdmqkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1hdlqhq</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Top coat chipping?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jf965bj8go6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1hdle3d</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Mid-peachy nude dupe?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdle3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1hdlbyq</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Metal Press-Ons?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdlbyq/metal_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1hdl9u3</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Took a gamble and happy to report I am one of the lucky ones that gets the purple shift. WHEW!!! Crisis averted..</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvky0glhco6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1hdl8is</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Quo brush replacement</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdl8is/quo_brush_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1hdl79l</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Mooncat Star Wars collab</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zdkwl5xbo6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1hdl2zp</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Cockadoodle Doom…obsessed</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kic2kqoyao6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1hdkwc0</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>House of Hades is sensory overload 😍</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdkwc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1hdjwok</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>All I see is red</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/BaGCtp8.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1hdjby6</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>ILNP Flicker</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdjby6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1hdjanh</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>ILNP black Friday mismatched skittle</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdjanh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1hcz8q8</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Lives up to the hype!</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hcz8q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1hdizn2</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Has anyone tried out this magnet?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdizn2/has_anyone_tried_out_this_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1hditx0</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Mooncat ups and downs</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hditx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1hdit2l</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Okay okay i can't resist any longer, heres my BF haul</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdit2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1hdiphi</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Tips for using peel-off base coat?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdiphi/tips_for_using_peeloff_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1hdig8y</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Clionadh Smedge Haze and cat tax</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdig8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1hdhx7a</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer Black Friday Haul</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdhx7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1hdhote</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Lack of sleep inspired this amateur attempt at holiday nails (feat. Nougat and Chocolate)</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrrt36vekn6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1hdhkga</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little underwhelmed by Blood Moon </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0n46dkbcjn6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1hdhdy8</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>🎄🎁Fighting Holiday Depression with Holiday Nails💅</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdhdy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1hdh4ig</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>This color rocks!!</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdh4ig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1hdh13r</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Is Sally Hansen GEL Primer the type you have to cure under a UV light?</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdh13r/is_sally_hansen_gel_primer_the_type_you_have_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1hdgjqu</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Feelin’ Festive</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdgjqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1hdgepi</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Inspired by other reindeers, I did my own!</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbgkzxtfan6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1hdg3px</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Warm and cozy sweater nails for a cold winter’s day </t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdg3px</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1hdf5v9</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Snowflakes! ❄️</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdf5v9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1hdf4q2</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Not taking any chances with my Mooncat bottles breaking!</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdf4q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1hdf2dt</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Product for 13 year old</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdf2dt/product_for_13_year_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1hdezgx</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How about this for a Christmas polish </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdezgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1hddjz8</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Emo for Life ft. Charlotte Brontë</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hddjz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1hdd7sa</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of the first polishes I mixed! </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdd7sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1hdd5q4</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Inspo: Christmas wrapping paper</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdd5q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1hdd1b0</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does Jewel Beetle work for a holiday party this weekend or would you change it to something more seasonal?! </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/grt6n4toim6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1hdbq1u</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Could someone Kleenex-swatch Chicago Fire and Cock a Doodle Doom for me?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdbq1u/could_someone_kleenexswatch_chicago_fire_and_cock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1hdb0i8</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>What is the least time consuming method of doing velvet style on magnetics?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdb0i8/what_is_the_least_time_consuming_method_of_doing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1hdankf</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Not sure they go together?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r9k9kz3vl6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1hd9dkd</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Classy red</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd9dkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1hd8mqo</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Those with skin conditions/dry skin, do you get irritation from doing nails?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hd8mqo/those_with_skin_conditionsdry_skin_do_you_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1hdv4os</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Tortoise Shell</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zklqr8ctq6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1hdsqn2</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Christmas Set</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdsqn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1hdsk6i</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Christmas nails!!!! ❄️☃️</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qn4gjl83q6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1hdrzp1</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Today ✨💜</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdrzp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1hdqf9l</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Pokémon</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdqf9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1hdp4y1</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I'm getting back into my love of nails.</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdp4y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1hdn1v7</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Christmas Nails! 🎄</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdn1v7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1hdlwtg</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I love my snow nails</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdlwtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1hdjwwx</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Any ideas?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyv898cl1o6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1hdjg1d</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspired by this sub! </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdjg1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1hdi5u2</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shout out to u/blairsmash for the tips. I can finally do plaid. </t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzncrhk1on6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1hdh62m</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>The practice set!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdh62m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1hdh41x</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>This is the first time I painted my nails red.</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4n2xuiufn6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1hdg062</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Miffy Nail Art! 🐰 </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdg062</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1hdbkak</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Christmas nails by Bea Beauty, Dublin, Ireland ❄️❤️❄️</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rohzp325m6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1hdag3q</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Pink Christmas anyone?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdag3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1hd7svq</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Noobie alert! Asked ChatGPT to design my nails</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hd7svq</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec 15 08:10:21 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_15.xlsx
+++ b/data/collected_data/2024_12_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1260"/>
+  <dimension ref="A1:C1452"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21854,6 +21854,3270 @@
         </is>
       </c>
     </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1hemo77</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Xmas nails!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/298mtupchy6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1hemmj5</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nice natural tone, I like the pink tone and you? </t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xb5wrmjrgy6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1hemczy</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>It's been ages since I tried a color that's not in the "natural" range.</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrcziueidy6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1hem94d</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Gel IQ oil remover?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hem94d/gel_iq_oil_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1helunj</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>How to make French tips last?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1helunj/how_to_make_french_tips_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1helafj</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Curing acrylic?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1helafj/curing_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1hel0p6</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>DND “Cherry Pie” with chrome</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7d9gqe15yx6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1hekzvw</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>My Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgbwb6cvxx6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1hek4kk</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Nail inspiration needed!!</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hek4kk/nail_inspiration_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1hee05m</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>My girl's nails!</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr9zhug62w6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1hedb4x</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Don’t like my nails :(</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hedb4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1heb4df</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snowy Night Sky 🌙 </t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heb4df</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1hecp7x</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">all of my nails are actually cracking like this. would you get hard gel or dip next? with nail health and integrity in mind. </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hecp7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1heas9v</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail split in the middle after hitting acrylic. </t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xb63diohbv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1he8cr6</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>GelX process made nails weak, advice for next time?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he8cr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1he63l1</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Nail tech reccos in the GTA?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1he63l1/nail_tech_reccos_in_the_gta/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1he2eo2</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Impress nails moving and irritate when I grab clothes or items</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8co8w73jbt6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1hdx5q5</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Did she fuck up my nail shaping or is my finger just weird?</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdx5q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1hdwzae</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Why do my nails keep falling off?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdwzae/why_do_my_nails_keep_falling_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1hdwvp7</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>My nails are severely damaged from me doing gel x at home - need suggestions on what to do?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ktfdib9dr6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1hekar5</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>BIAB starter kits (Canada)</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hekar5/biab_starter_kits_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1hekl5f</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Obsessed with my holiday nails!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hekl5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1hekbgb</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Before vs after exam week 😭</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hekbgb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1hejgfl</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>My boyfriend made me real copper metal nails</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hejgfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1hee3p2</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Got builder gel over frail nails after removing Gel X. Only 4 nails survive after 2 weeks…what should I do?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hee3p2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1hejusn</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>It’s the season ❄️☃️</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwn6resjlx6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1hehm7a</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Easy hack for brittle &amp; peeling nails: paint the underside too!</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hehm7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1heipkx</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Is this normal after a manicure?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mw0una2l9x6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1hejp43</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Gel nail stickers</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bg9t5c9wjx6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1hejp0f</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>What nails should I go with?</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hejp0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1hejhbq</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Christmas lights🎄✨️✨️</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hejhbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1heje2e</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Mooncat’s “Merkitten” 💕💖🧜🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4kect1qgx6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1hej711</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feelin’ Pine </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crlw1x9nex6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1heikt3</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY glitter dip powder for the holidays! </t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mipqui78x6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1heikhs</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on basics for tween? </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1heikhs/press_on_basics_for_tween/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1heidgl</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>DIY ombré.</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4iku4f76x6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1hei9y1</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>My Christmas set!! I love my girl Jessica bad ❤️‍🔥🎅🏻</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp4lszt75x6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1hehzs5</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>2024 nail recap</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hehzs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1hehodb</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Polygel Set Attempt</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjjz6o1azw6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1heh74c</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My take on Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heh74c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1hegn9j</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas ready 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/joukuvwkpw6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1hegmkc</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just HAVE to show people my nails </t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hegmkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1hegjwl</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>So proud I love them😭💕</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hegjwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1hegb0a</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Walking in a winter wonderland ❄️☃️</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnyo65jimw6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1hefrjr</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails for Holidays and new job Monday! </t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hefrjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1hefnxo</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try on nail art </t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3699i2kngw6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1hefh46</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decided to treat myself to a gel manicure today </t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejeq2zqyew6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1heeup3</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Festive season - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heeup3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1heefgk</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Is my manicure putting you in the New Year's mood</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xw382bp5w6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1heedd4</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>adventure time nails ⭑🐾₊˚⊹ ♡🐝</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heedd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1heecw3</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Party Tonight! </t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heecw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1hee4va</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter mint stiletto nails ❄️ </t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hee4va</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1hee4h8</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hee4h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1hedwy2</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>What is your take on fish nails?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hedwy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1hedlpi</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Took a pic before work, spent whole paycheck on getting mine and my Freind’s done</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hedlpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1hedkhu</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Fun with nail stickers!</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gg1j8wkyv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1hedkcl</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Peppermint Swirl 🎄</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1aihh12kyv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1hedik7</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Not sure about these</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/saxayjp5yv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1hedfkv</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>stupid question: how does nail salon pricing work?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hedfkv/stupid_question_how_does_nail_salon_pricing_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1hede0e</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Builder in a bottle and red Christmas mani. First time sharing a photo of my work :)</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5ykav94xv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1hecz9b</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Happy being a press on girly these days</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hecz9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1hecwyc</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9uw7i67tv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1hecr3n</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/387r2ppsrv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1hec188</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Do these look bad?</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2z61303ulv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1hebtvs</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY gel Mani that pretends to be natural nails </t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hebtvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1hebcoo</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>I haven't had a manicure in two years, I feel incredible now</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hebcoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1heb4a4</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday Nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heb4a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1heaqsr</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heaqsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1heaom5</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Blue winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eax62czqav6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1heagut</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Holiday sets I have done so far</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heagut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1he9xq2</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Ombré sparkle and pink Christmas nails ✨🎄</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he9xq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1he9uwb</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Tried chrome for the first time. 😊</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xt5z2qb24v6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1he9fv7</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>pre-christmas press-ons!</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he9fv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1he9bv7</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like this set? </t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftl8c1vrzu6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1he97p7</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I've been bamboozled!! </t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he97p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1he8sgi</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Timeless </t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hiu2uc9vu6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1he7y7s</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Bad nail break....help</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he7y7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1he7xc3</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>My simple Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he7xc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1he7vsk</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday nails! </t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtk3x26rnu6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1hdwqgn</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Nails no longer hold gel on</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hdwqgn/nails_no_longer_hold_gel_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1he7qn0</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Heart Nails 💕</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyfx98bjmu6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1he7jh9</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Luv so much how they turned out 💚🎄</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vf9h0cbuku6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1he7h04</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">need help </t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1he7h04/need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1he7csa</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Holiday ready with this fresh set💋🎄❄️</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dc1tkbaju6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1he729n</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kinda hate my nails. </t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he729n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1he6jdz</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Chisel Gel Cateye Dupe - Blue/Purple Shift</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8ghq5nfcu6e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1he6i43</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Got my nails done but I hate the color that I got, is there anything I can do?</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1he6i43/got_my_nails_done_but_i_hate_the_color_that_i_got/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1he2a45</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Should I let my nails breathe?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1he2a45/should_i_let_my_nails_breathe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1he2pbz</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>just some top coat ✨</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34mbi90ket6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1he65bc</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Nails did 💅</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fm2qnz69u6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1he64zs</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nieces nails that her 13 yo friend did! 50 USD. Definitely going to give her a try! </t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbvphfd49u6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1he55wn</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>my first winter set! (white chrome russian mani) ❄️</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he55wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1he55u3</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Merry Christmas ❄️</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he55u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1he50md</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter acrylic French [Male] </t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he50md</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1he4oga</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Painted my nails for a date but he cancelled. Still wanna show them off as I'm proud!</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb67cumowt6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1he40ux</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my new nails !! </t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he40ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1he3kn7</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Cranberry Jelly Nails</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he3kn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1he3gj4</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Dinner</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2w7p12xlt6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1he2z9j</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mvzwwz8ht6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1he2kgy</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Since I used kapping gel on my nails, the change was extraordinary, they grow super long and strong, I highly recommend it</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhgflav5dt6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1heo2cv</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>ILNP Evermore</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heo2cv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1heo1vw</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Christmas mani!</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heo1vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1hee2b3</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Sharing my polish collection + storage for fun! 🩷🧡💛💚💙💜</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hee2b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1he75s7</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>christmas nails!!</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he75s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1henfzf</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Holiday Skittle, But This Green…</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1henfzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1hem2ln</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails for my SIL’s wedding! </t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/royy4f83ay6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1helxil</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Luigi Mangione💖✨</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f6mynl7g8y6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1helfxe</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>monet water lilies dream set</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1helfau</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1hel505</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Recs for polish matching Nicole Loves Nails lipstick</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hel505/recs_for_polish_matching_nicole_loves_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1hekzg7</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Simple Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hekzg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1hekiej</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Has anyone had luck with fiber rubber base gel?</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hekiej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1hekhmr</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A few recent faves! </t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hekhmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1hek5t6</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>My new nailss 😍</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hek5t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1hek5kl</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>My new nailss 😍</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hek5kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1hejwlx</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Peppermint nails! (Pls ignore the messy nails)</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfmoauq2mx6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1hejrmu</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Psyche Minerals - Windy City Frost 😍</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hejrmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1hejp5h</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Linear holo + shimmer formula? </t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hejp5h/linear_holo_shimmer_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1hejg2l</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>there’s a miscoloured flakie in my sonic unicorn skin :0</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hejg2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1hej8yz</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>spirited away nail art !!</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hej8yz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1hej6i5</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>HOT TO GO</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ctbrfshex6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1heizej</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Comparison request: Holo Taco Playing With Sapphhire and FUN Lacquer Blue Tears</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1heizej/comparison_request_holo_taco_playing_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1heihu4</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>The Perfect Pearl?</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1heihu4/the_perfect_pearl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1heifc1</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>ILNP Lynb China Glaze</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heifc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1hei53e</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>✨Let it glow, ✨let glow, let it glow✨</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hei53e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1hehov2</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Another Fancy Gloss Thermal Appreciation Post</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hehov2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1hehm4h</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baby's first magnetic🧲 </t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9gjdaroyw6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1hehida</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Loving the Christmas tree vibe</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hehida</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1hegn92</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Panicking over seche!</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hegn92/panicking_over_seche/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1hegn69</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green glitter skittle swatches </t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzpeyf0kpw6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1hefnab</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Fun little 🧲 experiment:</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hefnab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1hefd8v</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>sculptural nails for me</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67i4wz80ew6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1heepdq</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Death Valley Bated Breath... OBSESSED</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heepdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1hedsu7</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>First Thermal</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hedsu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1hedpkq</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>The perfect Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc7bfcmqzv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1hedpfe</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>My mom's 14k gold nail from the 70's and my recreation in brass</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hedpfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1hedlag</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Gingerbread Cookie Art❄️</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hedlag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1hed4jd</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Essie Special Effects - Separated Starlight</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8tr0lovuv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1hecp3l</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Essie sent me a free gift 👀😂</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq23wbecrv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1hecinm</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone said I was obsessed with my hands. I really dk what they mean </t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtwav1jupv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1headaf</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>it's true what they say about fields of lavender!</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibburre38v6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1hea4lr</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>ILNP mega (S) as topcoat?</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hea4lr/ilnp_mega_s_as_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1he9wps</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Another sparkly red for the holidays? Groundbreaking. 😐</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he9wps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1he9rbd</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Literally cannot stop staring </t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he9rbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1he94sc</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Anyone else have this experience with Death Valley Nails?</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he94sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1he8x7r</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Happy Holidays ✨</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jtbmg1ewu6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1he8t1w</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>A Manicure to Compliment That Cashmere Sweater or Ugly Christmas Sweater</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmltxdxdvu6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1he8r09</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>In your opinion, what is the most overrated polish you’ve seen this year?</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88j44nnwuu6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1he8e7l</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Feeling Festive! 🎄</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he8e7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1he7y48</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>shifty and iridescent enough to distract me all day</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvve49vaou6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1he7vod</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone know about Yokefellow gel? Saw an ad, don't want to get scammed </t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1he7vod/anyone_know_about_yokefellow_gel_saw_an_ad_dont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1he7ong</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art for a holiday party</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucyl0772mu6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1he7lrr</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Got my Black Friday haul so I made my BF pick out a shade</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he7lrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1he7e3u</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Holidays nails!</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he7e3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1he6pu0</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Dense gold flakie?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1he6pu0/dense_gold_flakie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1he6m2q</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Been searching for colors like these but don't want to buy from Lights Lacquer </t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he6m2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1he6ijz</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Chisel Gel Cateye Dupe - Blue/Purple Shift</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1he6ijz/chisel_gel_cateye_dupe_bluepurple_shift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1he6cwg</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my partner loves this color but its sold out! any good matches you know? </t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4girh9yau6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1he5kpl</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>ILNP Pawprint</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04t7jqse4u6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1he537t</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Best brownish pinks?</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he537t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1he52d7</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Difference between indie vs mainstream polishes?</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1he52d7/difference_between_indie_vs_mainstream_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1he4yiz</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Ulta Strikes Again - cross posting in case it helps others</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he4wgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1he4986</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Labelling swatch sticks</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1he4986/labelling_swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1he3srv</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Stained Glass Palate Cleanser Nails</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3a91cqnyot6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1he3p4z</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My collection for your appreciation </t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he3p4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1he3g8p</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>I absolutely adore holos ✨️</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he3g8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1he1w2v</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Another Person in STEM with Glitter Nails!</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1he1w2v/another_person_in_stem_with_glitter_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1he15do</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Head In Clouds</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he15do</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1hdt6cn</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Gel top coat on Essie speed setter?</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdt6cn/gel_top_coat_on_essie_speed_setter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1hdtson</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Best top coat for nail art and charms similar to Seche Vite</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdtson/best_top_coat_for_nail_art_and_charms_similar_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1he0o8o</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Christmas mani tax</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he0o8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1hdyljb</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Can a glitter gel topcoat be used as a replacement for a normal gel topcoat</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hdyljb/can_a_glitter_gel_topcoat_be_used_as_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1he010f</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Berrylicious Golden Flakie </t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he010f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1hdzq7e</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>I have a type</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdzq7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1hdzopv</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>My 3YO said these were “too sparkly”!</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymhuh4fzcs6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1hdzemz</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Can someone help me understand colour theory?</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hdzemz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1hemig5</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>What do you think? Finish myself this morning hoho 2h of work. Thanks to my lil sis's feet</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnirpyrmey6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1hel726</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Some festive nails I just dif</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hel726</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1he7e86</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jq592erlju6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1hehq9a</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Blue winter gnome nails 😍</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pe7qvmlszw6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1heg00x</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>My first attempt at 3D</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zcobcxvrjw6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1hefrc3</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>opinions and criticism on my chrirstmas set?</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hefrc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1heffb2</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Some of the 151 set I’m gonna do</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heffb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1hef6ar</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>How do these pressons I made look?</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/848e1bzbcw6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1hef01g</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Uñas Navideñas que realicé el día hoy</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1w7nc2law6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1heevqi</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>What do you guys think of my nails</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9v0yhwws9w6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1heee17</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>i made some adventure time nails! ˚⊹ ♡🐝</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1heee17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1hedv5r</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Festive season - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hedv5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1hedotc</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>I can't tell if I like my nails or not</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1qanjpkzv6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1he7uyj</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails I made for myself. Constructive feedback appreciated. </t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he7uyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1he71og</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>A bit out of season but I got new stamping stencils and wanted to try them out - Fall press ons</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1he71og</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1he1n5c</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>Literally just two little guys</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y5myv4gr2t6e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1hdzpdm</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>POW! Set :-)</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5591xm98ds6e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>